<commit_message>
budapest es publik cimek kesz
</commit_message>
<xml_diff>
--- a/cimzes.xlsx
+++ b/cimzes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!Háló technikum\!vizsgaremek_sajat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F2FBB4-E0D7-4686-82EC-D4760CCD76D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60440A19-2BAA-4F59-AFC4-4460965F190F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6555" yWindow="7815" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{529DAD9C-076A-4599-B150-D0A99A7074A7}"/>
+    <workbookView xWindow="17370" yWindow="1665" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{529DAD9C-076A-4599-B150-D0A99A7074A7}"/>
   </bookViews>
   <sheets>
     <sheet name="BP" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="160">
   <si>
     <t>vlan 10</t>
   </si>
@@ -146,15 +146,6 @@
     <t>admin
 infobiztonság
 management vlan</t>
-  </si>
-  <si>
-    <t>quest wifi</t>
-  </si>
-  <si>
-    <t>quest 1</t>
-  </si>
-  <si>
-    <t>quest 2</t>
   </si>
   <si>
     <t>vlan 70</t>
@@ -310,12 +301,330 @@
   <si>
     <t>14.0.0.0</t>
   </si>
+  <si>
+    <t>172.16.0.0</t>
+  </si>
+  <si>
+    <t>172.16.0.1</t>
+  </si>
+  <si>
+    <t>172.16.1.254</t>
+  </si>
+  <si>
+    <t>172.16.1.255</t>
+  </si>
+  <si>
+    <t>./23</t>
+  </si>
+  <si>
+    <t>255.255.254.0</t>
+  </si>
+  <si>
+    <t>172.16.2.0</t>
+  </si>
+  <si>
+    <t>172.16.2.1</t>
+  </si>
+  <si>
+    <t>172.16.3.254</t>
+  </si>
+  <si>
+    <t>172.16.3.255</t>
+  </si>
+  <si>
+    <t>172.16.4.0</t>
+  </si>
+  <si>
+    <t>172.16.4.1</t>
+  </si>
+  <si>
+    <t>172.16.4.254</t>
+  </si>
+  <si>
+    <t>172.16.4.255</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>./24</t>
+  </si>
+  <si>
+    <t>172.16.5.0</t>
+  </si>
+  <si>
+    <t>172.16.5.1</t>
+  </si>
+  <si>
+    <t>172.16.5.254</t>
+  </si>
+  <si>
+    <t>172.16.5.255</t>
+  </si>
+  <si>
+    <t>172.16.6.0</t>
+  </si>
+  <si>
+    <t>172.16.6.1</t>
+  </si>
+  <si>
+    <t>172.16.6.126</t>
+  </si>
+  <si>
+    <t>172.16.6.127</t>
+  </si>
+  <si>
+    <t>255.255.255.128</t>
+  </si>
+  <si>
+    <t>./26</t>
+  </si>
+  <si>
+    <t>172.16.6.128</t>
+  </si>
+  <si>
+    <t>172.16.6.129</t>
+  </si>
+  <si>
+    <t>172.16.6.254</t>
+  </si>
+  <si>
+    <t>172.16.6.255</t>
+  </si>
+  <si>
+    <t>172.16.6.190</t>
+  </si>
+  <si>
+    <t>172.16.6.191</t>
+  </si>
+  <si>
+    <t>255.255.255.192</t>
+  </si>
+  <si>
+    <t>./25</t>
+  </si>
+  <si>
+    <t>172.16.6.192</t>
+  </si>
+  <si>
+    <t>172.16.6.193</t>
+  </si>
+  <si>
+    <t>172.16.7.62</t>
+  </si>
+  <si>
+    <t>172.16.7.63</t>
+  </si>
+  <si>
+    <t>172.16.7.0</t>
+  </si>
+  <si>
+    <t>172.16.7.1</t>
+  </si>
+  <si>
+    <t>172.16.7.64</t>
+  </si>
+  <si>
+    <t>172.16.7.65</t>
+  </si>
+  <si>
+    <t>172.16.7.126</t>
+  </si>
+  <si>
+    <t>172.16.7.127</t>
+  </si>
+  <si>
+    <t>172.16.7.128</t>
+  </si>
+  <si>
+    <t>172.16.7.129</t>
+  </si>
+  <si>
+    <t>172.16.7.190</t>
+  </si>
+  <si>
+    <t>172.16.7.191</t>
+  </si>
+  <si>
+    <t>172.16.7.158</t>
+  </si>
+  <si>
+    <t>172.16.7.159</t>
+  </si>
+  <si>
+    <t>255.255.255.224</t>
+  </si>
+  <si>
+    <t>./27</t>
+  </si>
+  <si>
+    <t>172.16.7.160</t>
+  </si>
+  <si>
+    <t>172.16.7.161</t>
+  </si>
+  <si>
+    <t>172.16.7.192</t>
+  </si>
+  <si>
+    <t>172.16.7.193</t>
+  </si>
+  <si>
+    <t>172.16.7.206</t>
+  </si>
+  <si>
+    <t>172.16.7.207</t>
+  </si>
+  <si>
+    <t>255.255.255.240</t>
+  </si>
+  <si>
+    <t>./28</t>
+  </si>
+  <si>
+    <t>172.16.7.208</t>
+  </si>
+  <si>
+    <t>172.16.7.209</t>
+  </si>
+  <si>
+    <t>172.16.7.222</t>
+  </si>
+  <si>
+    <t>172.16.7.223</t>
+  </si>
+  <si>
+    <t>255.255.255.252</t>
+  </si>
+  <si>
+    <t>./30</t>
+  </si>
+  <si>
+    <t>172.16.7.224</t>
+  </si>
+  <si>
+    <t>172.16.7.225</t>
+  </si>
+  <si>
+    <t>172.16.7.226</t>
+  </si>
+  <si>
+    <t>172.16.7.227</t>
+  </si>
+  <si>
+    <t>172.16.7.228</t>
+  </si>
+  <si>
+    <t>172.16.7.232</t>
+  </si>
+  <si>
+    <t>172.16.7.236</t>
+  </si>
+  <si>
+    <t>172.16.7.240</t>
+  </si>
+  <si>
+    <t>172.16.7.244</t>
+  </si>
+  <si>
+    <t>172.16.7.229</t>
+  </si>
+  <si>
+    <t>172.16.7.230</t>
+  </si>
+  <si>
+    <t>172.16.7.231</t>
+  </si>
+  <si>
+    <t>172.16.7.233</t>
+  </si>
+  <si>
+    <t>172.16.7.234</t>
+  </si>
+  <si>
+    <t>172.16.7.235</t>
+  </si>
+  <si>
+    <t>172.16.7.237</t>
+  </si>
+  <si>
+    <t>172.16.7.238</t>
+  </si>
+  <si>
+    <t>172.16.7.239</t>
+  </si>
+  <si>
+    <t>172.16.7.241</t>
+  </si>
+  <si>
+    <t>172.16.7.242</t>
+  </si>
+  <si>
+    <t>172.16.7.243</t>
+  </si>
+  <si>
+    <t>172.16.7.245</t>
+  </si>
+  <si>
+    <t>172.16.7.246</t>
+  </si>
+  <si>
+    <t>172.16.7.247</t>
+  </si>
+  <si>
+    <t>11.0.0.1</t>
+  </si>
+  <si>
+    <t>11.0.0.2</t>
+  </si>
+  <si>
+    <t>11.0.0.3</t>
+  </si>
+  <si>
+    <t>12.0.0.1</t>
+  </si>
+  <si>
+    <t>12.0.0.2</t>
+  </si>
+  <si>
+    <t>12.0.0.3</t>
+  </si>
+  <si>
+    <t>13.0.0.1</t>
+  </si>
+  <si>
+    <t>13.0.0.2</t>
+  </si>
+  <si>
+    <t>13.0.0.3</t>
+  </si>
+  <si>
+    <t>14.0.0.1</t>
+  </si>
+  <si>
+    <t>14.0.0.2</t>
+  </si>
+  <si>
+    <t>14.0.0.3</t>
+  </si>
+  <si>
+    <t>wifi</t>
+  </si>
+  <si>
+    <t>guest 1</t>
+  </si>
+  <si>
+    <t>guest 2</t>
+  </si>
+  <si>
+    <t>guest wifi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,6 +645,13 @@
       <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -690,7 +1006,7 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,14 +1019,20 @@
     <col min="8" max="8" width="15.140625" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" customWidth="1"/>
     <col min="10" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -734,10 +1056,10 @@
     </row>
     <row r="2" spans="1:20" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>37</v>
+        <v>157</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>158</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>15</v>
@@ -802,16 +1124,16 @@
         <v>4</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L3" t="s">
         <v>5</v>
       </c>
       <c r="M3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="N3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="O3" t="s">
         <v>7</v>
@@ -898,6 +1220,12 @@
       <c r="A5" t="s">
         <v>13</v>
       </c>
+      <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>156</v>
+      </c>
       <c r="D5">
         <v>230</v>
       </c>
@@ -954,36 +1282,379 @@
       <c r="A6" t="s">
         <v>28</v>
       </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M6" t="s">
+        <v>108</v>
+      </c>
+      <c r="N6" t="s">
+        <v>114</v>
+      </c>
+      <c r="O6" t="s">
+        <v>120</v>
+      </c>
+      <c r="P6" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>125</v>
+      </c>
+      <c r="R6" t="s">
+        <v>126</v>
+      </c>
+      <c r="S6" t="s">
+        <v>127</v>
+      </c>
+      <c r="T6" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" t="s">
+        <v>95</v>
+      </c>
+      <c r="K7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L7" t="s">
+        <v>107</v>
+      </c>
+      <c r="M7" t="s">
+        <v>109</v>
+      </c>
+      <c r="N7" t="s">
+        <v>115</v>
+      </c>
+      <c r="O7" t="s">
+        <v>121</v>
+      </c>
+      <c r="P7" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>132</v>
+      </c>
+      <c r="R7" t="s">
+        <v>135</v>
+      </c>
+      <c r="S7" t="s">
+        <v>138</v>
+      </c>
+      <c r="T7" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" t="s">
+        <v>96</v>
+      </c>
+      <c r="K8" t="s">
+        <v>102</v>
+      </c>
+      <c r="L8" t="s">
+        <v>100</v>
+      </c>
+      <c r="M8" t="s">
+        <v>110</v>
+      </c>
+      <c r="N8" t="s">
+        <v>116</v>
+      </c>
+      <c r="O8" t="s">
+        <v>122</v>
+      </c>
+      <c r="P8" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>133</v>
+      </c>
+      <c r="R8" t="s">
+        <v>136</v>
+      </c>
+      <c r="S8" t="s">
+        <v>139</v>
+      </c>
+      <c r="T8" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" t="s">
+        <v>103</v>
+      </c>
+      <c r="L9" t="s">
+        <v>101</v>
+      </c>
+      <c r="M9" t="s">
+        <v>111</v>
+      </c>
+      <c r="N9" t="s">
+        <v>117</v>
+      </c>
+      <c r="O9" t="s">
+        <v>123</v>
+      </c>
+      <c r="P9" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>134</v>
+      </c>
+      <c r="R9" t="s">
+        <v>137</v>
+      </c>
+      <c r="S9" t="s">
+        <v>140</v>
+      </c>
+      <c r="T9" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" t="s">
+        <v>104</v>
+      </c>
+      <c r="L10" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10" t="s">
+        <v>112</v>
+      </c>
+      <c r="N10" t="s">
+        <v>112</v>
+      </c>
+      <c r="O10" t="s">
+        <v>118</v>
+      </c>
+      <c r="P10" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>118</v>
+      </c>
+      <c r="R10" t="s">
+        <v>118</v>
+      </c>
+      <c r="S10" t="s">
+        <v>118</v>
+      </c>
+      <c r="T10" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" t="s">
+        <v>79</v>
+      </c>
+      <c r="K11" t="s">
+        <v>105</v>
+      </c>
+      <c r="L11" t="s">
+        <v>105</v>
+      </c>
+      <c r="M11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N11" t="s">
+        <v>113</v>
+      </c>
+      <c r="O11" t="s">
+        <v>119</v>
+      </c>
+      <c r="P11" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>119</v>
+      </c>
+      <c r="R11" t="s">
+        <v>119</v>
+      </c>
+      <c r="S11" t="s">
+        <v>119</v>
+      </c>
+      <c r="T11" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:T1"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -994,7 +1665,7 @@
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1675,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1027,7 +1698,7 @@
     </row>
     <row r="2" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>36</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -1092,13 +1763,13 @@
         <v>4</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L3" t="s">
         <v>5</v>
       </c>
       <c r="M3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N3" t="s">
         <v>7</v>
@@ -1222,7 +1893,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1232,7 +1903,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" t="s">
@@ -1242,7 +1913,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1323,16 +1994,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1343,7 +2014,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,7 +2026,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1364,79 +2035,176 @@
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>48</v>
       </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
         <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
+      <c r="B7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
+      <c r="B8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
+      <c r="B9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>